<commit_message>
Update ERM, doc and decision matrix
</commit_message>
<xml_diff>
--- a/doc/decision_matrix.xlsx
+++ b/doc/decision_matrix.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.gaechter\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.gaechter\git\hub\arbeitszeitserfassung_wohnen\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3E1BC4-551C-46E1-BA0E-766FBC8F6CE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DB13FC-25F8-4A89-8CCF-E0BB06612768}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{456824B9-6D9D-4D45-82D7-803A7CA47132}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Zeitklasse" sheetId="1" r:id="rId1"/>
+    <sheet name="Zeitzone festlegen" sheetId="2" r:id="rId2"/>
+    <sheet name="Curl PHP oder Symfony " sheetId="3" r:id="rId3"/>
+    <sheet name="Kontroller Bereiche " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Kategorie</t>
   </si>
@@ -52,23 +55,34 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Zentral</t>
+  </si>
+  <si>
+    <t>Meheren Orten</t>
+  </si>
+  <si>
+    <t>Fehleranfälligkeit</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>Symfony</t>
+  </si>
+  <si>
+    <t>Redundanz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,8 +122,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -427,7 +441,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -494,7 +508,7 @@
       </c>
       <c r="B5">
         <f>B2*E2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <f>C2*E2</f>
@@ -527,7 +541,7 @@
       </c>
       <c r="B8" s="1">
         <f>SUM(B5:B7)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2">
         <f>SUM(C5:C7)</f>
@@ -537,4 +551,281 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7784446-BA92-4FC1-A5DB-B1AEEEE82A09}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f>B2*E2</f>
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <f>C2*E2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>B3*E3</f>
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <f>C3*E3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>B4*E4</f>
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f>C4*E4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>B5*E5</f>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>C5*E5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <f>SUM(B6:B9)</f>
+        <v>44</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUM(C6:C9)</f>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE006A-BE93-4C5A-9651-D6A19062C0FB}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>B2*E2</f>
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f>C2*E2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" ref="B6:B7" si="0">B3*E3</f>
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C7" si="1">C3*E3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <f>SUM(B5:B7)</f>
+        <v>30</v>
+      </c>
+      <c r="C8" s="2">
+        <f>SUM(C5:C7)</f>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC286E4-4039-4DA7-8565-83AF48E349BE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>